<commit_message>
Add sum_chromosomes stats in export
Update statistics algorithm to delete the 5 useless hashmaps
Update CDSResult constructor to initialize the hashmaps
</commit_message>
<xml_diff>
--- a/intelliji/resources/template.xlsx
+++ b/intelliji/resources/template.xlsx
@@ -53,7 +53,7 @@
     <t xml:space="preserve">Nombre d’organismes</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre CDS du fichier</t>
+    <t xml:space="preserve">Nombre total de CDS</t>
   </si>
   <si>
     <r>
@@ -861,10 +861,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -943,23 +945,25 @@
   <dimension ref="A1:Q76"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="9.86224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.86224489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.9489795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2960,7 +2964,7 @@
       <c r="I75" s="25"/>
       <c r="J75" s="25"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="33" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Increase size of columns in template
</commit_message>
<xml_diff>
--- a/intelliji/resources/template.xlsx
+++ b/intelliji/resources/template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="General_Information" sheetId="1" r:id="rId1"/>
@@ -660,12 +660,6 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -676,6 +670,12 @@
     <xf numFmtId="2" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="11" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1114,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1123,15 +1123,14 @@
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.85546875"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.140625"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.85546875"/>
-    <col min="8" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="8" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="8.5703125"/>
-    <col min="12" max="12" width="22.28515625"/>
-    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" customWidth="1"/>
@@ -1142,10 +1141,10 @@
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -1177,20 +1176,20 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
@@ -1200,16 +1199,16 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
@@ -1222,16 +1221,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
@@ -1241,16 +1240,16 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
@@ -1263,16 +1262,16 @@
         <v>0</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
@@ -1409,34 +1408,34 @@
       <c r="A13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29" t="str">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="str">
         <f t="shared" ref="C13:C44" si="0">IFERROR(B13/$B$77*100,"")</f>
         <v/>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="30" t="str">
+      <c r="D13" s="26"/>
+      <c r="E13" s="28" t="str">
         <f t="shared" ref="E13:E44" si="1">IFERROR(D13/$D$77*100,"")</f>
         <v/>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="30" t="str">
+      <c r="F13" s="26"/>
+      <c r="G13" s="28" t="str">
         <f t="shared" ref="G13:G44" si="2">IFERROR(F13/$F$77*100,"")</f>
         <v/>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
       <c r="L13" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="34"/>
-      <c r="N13" s="35" t="str">
+      <c r="M13" s="32"/>
+      <c r="N13" s="33" t="str">
         <f t="shared" ref="N13:N28" si="3">IFERROR(M13/$M$29*100,"")</f>
         <v/>
       </c>
-      <c r="O13" s="34"/>
-      <c r="P13" s="35" t="str">
+      <c r="O13" s="32"/>
+      <c r="P13" s="33" t="str">
         <f t="shared" ref="P13:P28" si="4">IFERROR(O13/$O$29*100,"")</f>
         <v/>
       </c>
@@ -1445,34 +1444,34 @@
       <c r="A14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="32" t="str">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="33" t="str">
+      <c r="D14" s="29"/>
+      <c r="E14" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="33" t="str">
+      <c r="F14" s="29"/>
+      <c r="G14" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
       <c r="L14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="36"/>
-      <c r="N14" s="37" t="str">
+      <c r="M14" s="34"/>
+      <c r="N14" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O14" s="36"/>
-      <c r="P14" s="37" t="str">
+      <c r="O14" s="34"/>
+      <c r="P14" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1481,34 +1480,34 @@
       <c r="A15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29" t="str">
+      <c r="B15" s="26"/>
+      <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="30" t="str">
+      <c r="D15" s="26"/>
+      <c r="E15" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="30" t="str">
+      <c r="F15" s="26"/>
+      <c r="G15" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
       <c r="L15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="34"/>
-      <c r="N15" s="35" t="str">
+      <c r="M15" s="32"/>
+      <c r="N15" s="33" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O15" s="34"/>
-      <c r="P15" s="35" t="str">
+      <c r="O15" s="32"/>
+      <c r="P15" s="33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1517,34 +1516,34 @@
       <c r="A16" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32" t="str">
+      <c r="B16" s="29"/>
+      <c r="C16" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="33" t="str">
+      <c r="D16" s="29"/>
+      <c r="E16" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="33" t="str">
+      <c r="F16" s="29"/>
+      <c r="G16" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
       <c r="L16" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="36"/>
-      <c r="N16" s="37" t="str">
+      <c r="M16" s="34"/>
+      <c r="N16" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O16" s="36"/>
-      <c r="P16" s="37" t="str">
+      <c r="O16" s="34"/>
+      <c r="P16" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1553,34 +1552,34 @@
       <c r="A17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29" t="str">
+      <c r="B17" s="26"/>
+      <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="30" t="str">
+      <c r="D17" s="26"/>
+      <c r="E17" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="30" t="str">
+      <c r="F17" s="26"/>
+      <c r="G17" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
       <c r="L17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="M17" s="34"/>
-      <c r="N17" s="35" t="str">
+      <c r="M17" s="32"/>
+      <c r="N17" s="33" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O17" s="34"/>
-      <c r="P17" s="35" t="str">
+      <c r="O17" s="32"/>
+      <c r="P17" s="33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1589,34 +1588,34 @@
       <c r="A18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32" t="str">
+      <c r="B18" s="29"/>
+      <c r="C18" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="33" t="str">
+      <c r="D18" s="29"/>
+      <c r="E18" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="33" t="str">
+      <c r="F18" s="29"/>
+      <c r="G18" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
       <c r="L18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M18" s="36"/>
-      <c r="N18" s="37" t="str">
+      <c r="M18" s="34"/>
+      <c r="N18" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O18" s="36"/>
-      <c r="P18" s="37" t="str">
+      <c r="O18" s="34"/>
+      <c r="P18" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1625,34 +1624,34 @@
       <c r="A19" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29" t="str">
+      <c r="B19" s="26"/>
+      <c r="C19" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="30" t="str">
+      <c r="D19" s="26"/>
+      <c r="E19" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="30" t="str">
+      <c r="F19" s="26"/>
+      <c r="G19" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
       <c r="L19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M19" s="34"/>
-      <c r="N19" s="35" t="str">
+      <c r="M19" s="32"/>
+      <c r="N19" s="33" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O19" s="34"/>
-      <c r="P19" s="35" t="str">
+      <c r="O19" s="32"/>
+      <c r="P19" s="33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1661,34 +1660,34 @@
       <c r="A20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32" t="str">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="33" t="str">
+      <c r="D20" s="29"/>
+      <c r="E20" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="33" t="str">
+      <c r="F20" s="29"/>
+      <c r="G20" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
       <c r="L20" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="M20" s="36"/>
-      <c r="N20" s="37" t="str">
+      <c r="M20" s="34"/>
+      <c r="N20" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O20" s="36"/>
-      <c r="P20" s="37" t="str">
+      <c r="O20" s="34"/>
+      <c r="P20" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1697,34 +1696,34 @@
       <c r="A21" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29" t="str">
+      <c r="B21" s="26"/>
+      <c r="C21" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="30" t="str">
+      <c r="D21" s="26"/>
+      <c r="E21" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="30" t="str">
+      <c r="F21" s="26"/>
+      <c r="G21" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
       <c r="L21" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M21" s="34"/>
-      <c r="N21" s="35" t="str">
+      <c r="M21" s="32"/>
+      <c r="N21" s="33" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O21" s="34"/>
-      <c r="P21" s="35" t="str">
+      <c r="O21" s="32"/>
+      <c r="P21" s="33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1733,34 +1732,34 @@
       <c r="A22" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32" t="str">
+      <c r="B22" s="29"/>
+      <c r="C22" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="33" t="str">
+      <c r="D22" s="29"/>
+      <c r="E22" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="33" t="str">
+      <c r="F22" s="29"/>
+      <c r="G22" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
       <c r="L22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M22" s="36"/>
-      <c r="N22" s="37" t="str">
+      <c r="M22" s="34"/>
+      <c r="N22" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O22" s="36"/>
-      <c r="P22" s="37" t="str">
+      <c r="O22" s="34"/>
+      <c r="P22" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1769,34 +1768,34 @@
       <c r="A23" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29" t="str">
+      <c r="B23" s="26"/>
+      <c r="C23" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="30" t="str">
+      <c r="D23" s="26"/>
+      <c r="E23" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="30" t="str">
+      <c r="F23" s="26"/>
+      <c r="G23" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
       <c r="L23" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="M23" s="34"/>
-      <c r="N23" s="35" t="str">
+      <c r="M23" s="32"/>
+      <c r="N23" s="33" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O23" s="34"/>
-      <c r="P23" s="35" t="str">
+      <c r="O23" s="32"/>
+      <c r="P23" s="33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1805,34 +1804,34 @@
       <c r="A24" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32" t="str">
+      <c r="B24" s="29"/>
+      <c r="C24" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="33" t="str">
+      <c r="D24" s="29"/>
+      <c r="E24" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="33" t="str">
+      <c r="F24" s="29"/>
+      <c r="G24" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
       <c r="L24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="M24" s="36"/>
-      <c r="N24" s="37" t="str">
+      <c r="M24" s="34"/>
+      <c r="N24" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O24" s="36"/>
-      <c r="P24" s="37" t="str">
+      <c r="O24" s="34"/>
+      <c r="P24" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1841,34 +1840,34 @@
       <c r="A25" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29" t="str">
+      <c r="B25" s="26"/>
+      <c r="C25" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="30" t="str">
+      <c r="D25" s="26"/>
+      <c r="E25" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="30" t="str">
+      <c r="F25" s="26"/>
+      <c r="G25" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
       <c r="L25" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="M25" s="34"/>
-      <c r="N25" s="35" t="str">
+      <c r="M25" s="32"/>
+      <c r="N25" s="33" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O25" s="34"/>
-      <c r="P25" s="35" t="str">
+      <c r="O25" s="32"/>
+      <c r="P25" s="33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1877,34 +1876,34 @@
       <c r="A26" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32" t="str">
+      <c r="B26" s="29"/>
+      <c r="C26" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="33" t="str">
+      <c r="D26" s="29"/>
+      <c r="E26" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="33" t="str">
+      <c r="F26" s="29"/>
+      <c r="G26" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
       <c r="L26" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="M26" s="36"/>
-      <c r="N26" s="37" t="str">
+      <c r="M26" s="34"/>
+      <c r="N26" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O26" s="36"/>
-      <c r="P26" s="37" t="str">
+      <c r="O26" s="34"/>
+      <c r="P26" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1913,34 +1912,34 @@
       <c r="A27" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29" t="str">
+      <c r="B27" s="26"/>
+      <c r="C27" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="30" t="str">
+      <c r="D27" s="26"/>
+      <c r="E27" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="30" t="str">
+      <c r="F27" s="26"/>
+      <c r="G27" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
       <c r="L27" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="M27" s="34"/>
-      <c r="N27" s="35" t="str">
+      <c r="M27" s="32"/>
+      <c r="N27" s="33" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O27" s="34"/>
-      <c r="P27" s="35" t="str">
+      <c r="O27" s="32"/>
+      <c r="P27" s="33" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1949,34 +1948,34 @@
       <c r="A28" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32" t="str">
+      <c r="B28" s="29"/>
+      <c r="C28" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="33" t="str">
+      <c r="D28" s="29"/>
+      <c r="E28" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="33" t="str">
+      <c r="F28" s="29"/>
+      <c r="G28" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
       <c r="L28" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="M28" s="36"/>
-      <c r="N28" s="37" t="str">
+      <c r="M28" s="34"/>
+      <c r="N28" s="35" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O28" s="36"/>
-      <c r="P28" s="37" t="str">
+      <c r="O28" s="34"/>
+      <c r="P28" s="35" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -1985,24 +1984,24 @@
       <c r="A29" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29" t="str">
+      <c r="B29" s="26"/>
+      <c r="C29" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="30" t="str">
+      <c r="D29" s="26"/>
+      <c r="E29" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="30" t="str">
+      <c r="F29" s="26"/>
+      <c r="G29" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
       <c r="L29" s="19" t="s">
         <v>65</v>
       </c>
@@ -2027,70 +2026,70 @@
       <c r="A30" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="32" t="str">
+      <c r="B30" s="29"/>
+      <c r="C30" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="33" t="str">
+      <c r="D30" s="29"/>
+      <c r="E30" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="33" t="str">
+      <c r="F30" s="29"/>
+      <c r="G30" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
     </row>
     <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29" t="str">
+      <c r="B31" s="26"/>
+      <c r="C31" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="30" t="str">
+      <c r="D31" s="26"/>
+      <c r="E31" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F31" s="28"/>
-      <c r="G31" s="30" t="str">
+      <c r="F31" s="26"/>
+      <c r="G31" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="32" t="str">
+      <c r="B32" s="29"/>
+      <c r="C32" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="33" t="str">
+      <c r="D32" s="29"/>
+      <c r="E32" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="33" t="str">
+      <c r="F32" s="29"/>
+      <c r="G32" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
@@ -2101,24 +2100,24 @@
       <c r="A33" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29" t="str">
+      <c r="B33" s="26"/>
+      <c r="C33" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="30" t="str">
+      <c r="D33" s="26"/>
+      <c r="E33" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F33" s="28"/>
-      <c r="G33" s="30" t="str">
+      <c r="F33" s="26"/>
+      <c r="G33" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
       <c r="L33" s="21"/>
       <c r="M33" s="21"/>
       <c r="N33" s="21"/>
@@ -2129,24 +2128,24 @@
       <c r="A34" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32" t="str">
+      <c r="B34" s="29"/>
+      <c r="C34" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="33" t="str">
+      <c r="D34" s="29"/>
+      <c r="E34" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="33" t="str">
+      <c r="F34" s="29"/>
+      <c r="G34" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
@@ -2157,24 +2156,24 @@
       <c r="A35" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29" t="str">
+      <c r="B35" s="26"/>
+      <c r="C35" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D35" s="28"/>
-      <c r="E35" s="30" t="str">
+      <c r="D35" s="26"/>
+      <c r="E35" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="30" t="str">
+      <c r="F35" s="26"/>
+      <c r="G35" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
       <c r="L35" s="21"/>
       <c r="M35" s="21"/>
       <c r="N35" s="21"/>
@@ -2185,24 +2184,24 @@
       <c r="A36" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="32" t="str">
+      <c r="B36" s="29"/>
+      <c r="C36" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="33" t="str">
+      <c r="D36" s="29"/>
+      <c r="E36" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="33" t="str">
+      <c r="F36" s="29"/>
+      <c r="G36" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
@@ -2213,24 +2212,24 @@
       <c r="A37" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29" t="str">
+      <c r="B37" s="26"/>
+      <c r="C37" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="30" t="str">
+      <c r="D37" s="26"/>
+      <c r="E37" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F37" s="28"/>
-      <c r="G37" s="30" t="str">
+      <c r="F37" s="26"/>
+      <c r="G37" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
       <c r="L37" s="21"/>
       <c r="M37" s="21"/>
       <c r="N37" s="21"/>
@@ -2241,47 +2240,47 @@
       <c r="A38" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="32" t="str">
+      <c r="B38" s="29"/>
+      <c r="C38" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="33" t="str">
+      <c r="D38" s="29"/>
+      <c r="E38" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="33" t="str">
+      <c r="F38" s="29"/>
+      <c r="G38" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
     </row>
     <row r="39" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29" t="str">
+      <c r="B39" s="26"/>
+      <c r="C39" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="30" t="str">
+      <c r="D39" s="26"/>
+      <c r="E39" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F39" s="28"/>
-      <c r="G39" s="30" t="str">
+      <c r="F39" s="26"/>
+      <c r="G39" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
       <c r="M39" s="21"/>
       <c r="N39" s="21"/>
       <c r="O39" s="21"/>
@@ -2292,24 +2291,24 @@
       <c r="A40" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="32" t="str">
+      <c r="B40" s="29"/>
+      <c r="C40" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="33" t="str">
+      <c r="D40" s="29"/>
+      <c r="E40" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F40" s="31"/>
-      <c r="G40" s="33" t="str">
+      <c r="F40" s="29"/>
+      <c r="G40" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -2320,24 +2319,24 @@
       <c r="A41" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="29" t="str">
+      <c r="B41" s="26"/>
+      <c r="C41" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="30" t="str">
+      <c r="D41" s="26"/>
+      <c r="E41" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F41" s="28"/>
-      <c r="G41" s="30" t="str">
+      <c r="F41" s="26"/>
+      <c r="G41" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
@@ -2348,24 +2347,24 @@
       <c r="A42" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="32" t="str">
+      <c r="B42" s="29"/>
+      <c r="C42" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="33" t="str">
+      <c r="D42" s="29"/>
+      <c r="E42" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F42" s="31"/>
-      <c r="G42" s="33" t="str">
+      <c r="F42" s="29"/>
+      <c r="G42" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
@@ -2376,783 +2375,783 @@
       <c r="A43" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="29" t="str">
+      <c r="B43" s="26"/>
+      <c r="C43" s="27" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="30" t="str">
+      <c r="D43" s="26"/>
+      <c r="E43" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F43" s="28"/>
-      <c r="G43" s="30" t="str">
+      <c r="F43" s="26"/>
+      <c r="G43" s="28" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="32" t="str">
+      <c r="B44" s="29"/>
+      <c r="C44" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="33" t="str">
+      <c r="D44" s="29"/>
+      <c r="E44" s="31" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F44" s="31"/>
-      <c r="G44" s="33" t="str">
+      <c r="F44" s="29"/>
+      <c r="G44" s="31" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
     </row>
     <row r="45" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="29" t="str">
+      <c r="B45" s="26"/>
+      <c r="C45" s="27" t="str">
         <f t="shared" ref="C45:C76" si="5">IFERROR(B45/$B$77*100,"")</f>
         <v/>
       </c>
-      <c r="D45" s="28"/>
-      <c r="E45" s="30" t="str">
+      <c r="D45" s="26"/>
+      <c r="E45" s="28" t="str">
         <f t="shared" ref="E45:E76" si="6">IFERROR(D45/$D$77*100,"")</f>
         <v/>
       </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="30" t="str">
+      <c r="F45" s="26"/>
+      <c r="G45" s="28" t="str">
         <f t="shared" ref="G45:G76" si="7">IFERROR(F45/$F$77*100,"")</f>
         <v/>
       </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="32" t="str">
+      <c r="B46" s="29"/>
+      <c r="C46" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D46" s="31"/>
-      <c r="E46" s="33" t="str">
+      <c r="D46" s="29"/>
+      <c r="E46" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F46" s="31"/>
-      <c r="G46" s="33" t="str">
+      <c r="F46" s="29"/>
+      <c r="G46" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="28"/>
-      <c r="C47" s="29" t="str">
+      <c r="B47" s="26"/>
+      <c r="C47" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D47" s="28"/>
-      <c r="E47" s="30" t="str">
+      <c r="D47" s="26"/>
+      <c r="E47" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="30" t="str">
+      <c r="F47" s="26"/>
+      <c r="G47" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B48" s="31"/>
-      <c r="C48" s="32" t="str">
+      <c r="B48" s="29"/>
+      <c r="C48" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="33" t="str">
+      <c r="D48" s="29"/>
+      <c r="E48" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="33" t="str">
+      <c r="F48" s="29"/>
+      <c r="G48" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H48" s="31"/>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="29" t="str">
+      <c r="B49" s="26"/>
+      <c r="C49" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="30" t="str">
+      <c r="D49" s="26"/>
+      <c r="E49" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F49" s="28"/>
-      <c r="G49" s="30" t="str">
+      <c r="F49" s="26"/>
+      <c r="G49" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="32" t="str">
+      <c r="B50" s="29"/>
+      <c r="C50" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="33" t="str">
+      <c r="D50" s="29"/>
+      <c r="E50" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F50" s="31"/>
-      <c r="G50" s="33" t="str">
+      <c r="F50" s="29"/>
+      <c r="G50" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
     </row>
     <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="29" t="str">
+      <c r="B51" s="26"/>
+      <c r="C51" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D51" s="28"/>
-      <c r="E51" s="30" t="str">
+      <c r="D51" s="26"/>
+      <c r="E51" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F51" s="28"/>
-      <c r="G51" s="30" t="str">
+      <c r="F51" s="26"/>
+      <c r="G51" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H51" s="28"/>
-      <c r="I51" s="28"/>
-      <c r="J51" s="28"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="32" t="str">
+      <c r="B52" s="29"/>
+      <c r="C52" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D52" s="31"/>
-      <c r="E52" s="33" t="str">
+      <c r="D52" s="29"/>
+      <c r="E52" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F52" s="31"/>
-      <c r="G52" s="33" t="str">
+      <c r="F52" s="29"/>
+      <c r="G52" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
-      <c r="J52" s="31"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
     </row>
     <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="29" t="str">
+      <c r="B53" s="26"/>
+      <c r="C53" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D53" s="28"/>
-      <c r="E53" s="30" t="str">
+      <c r="D53" s="26"/>
+      <c r="E53" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F53" s="28"/>
-      <c r="G53" s="30" t="str">
+      <c r="F53" s="26"/>
+      <c r="G53" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H53" s="28"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="32" t="str">
+      <c r="B54" s="29"/>
+      <c r="C54" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D54" s="31"/>
-      <c r="E54" s="33" t="str">
+      <c r="D54" s="29"/>
+      <c r="E54" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F54" s="31"/>
-      <c r="G54" s="33" t="str">
+      <c r="F54" s="29"/>
+      <c r="G54" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
     </row>
     <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="28"/>
-      <c r="C55" s="29" t="str">
+      <c r="B55" s="26"/>
+      <c r="C55" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D55" s="28"/>
-      <c r="E55" s="30" t="str">
+      <c r="D55" s="26"/>
+      <c r="E55" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F55" s="28"/>
-      <c r="G55" s="30" t="str">
+      <c r="F55" s="26"/>
+      <c r="G55" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
-      <c r="J55" s="28"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="32" t="str">
+      <c r="B56" s="29"/>
+      <c r="C56" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D56" s="31"/>
-      <c r="E56" s="33" t="str">
+      <c r="D56" s="29"/>
+      <c r="E56" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F56" s="31"/>
-      <c r="G56" s="33" t="str">
+      <c r="F56" s="29"/>
+      <c r="G56" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-      <c r="J56" s="31"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="29" t="str">
+      <c r="B57" s="26"/>
+      <c r="C57" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D57" s="28"/>
-      <c r="E57" s="30" t="str">
+      <c r="D57" s="26"/>
+      <c r="E57" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F57" s="28"/>
-      <c r="G57" s="30" t="str">
+      <c r="F57" s="26"/>
+      <c r="G57" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H57" s="28"/>
-      <c r="I57" s="28"/>
-      <c r="J57" s="28"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
     </row>
     <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="31"/>
-      <c r="C58" s="32" t="str">
+      <c r="B58" s="29"/>
+      <c r="C58" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D58" s="31"/>
-      <c r="E58" s="33" t="str">
+      <c r="D58" s="29"/>
+      <c r="E58" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F58" s="31"/>
-      <c r="G58" s="33" t="str">
+      <c r="F58" s="29"/>
+      <c r="G58" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
-      <c r="J58" s="31"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="29"/>
     </row>
     <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="28"/>
-      <c r="C59" s="29" t="str">
+      <c r="B59" s="26"/>
+      <c r="C59" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D59" s="28"/>
-      <c r="E59" s="30" t="str">
+      <c r="D59" s="26"/>
+      <c r="E59" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="30" t="str">
+      <c r="F59" s="26"/>
+      <c r="G59" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
-      <c r="J59" s="28"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
     </row>
     <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="31"/>
-      <c r="C60" s="32" t="str">
+      <c r="B60" s="29"/>
+      <c r="C60" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D60" s="31"/>
-      <c r="E60" s="33" t="str">
+      <c r="D60" s="29"/>
+      <c r="E60" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F60" s="31"/>
-      <c r="G60" s="33" t="str">
+      <c r="F60" s="29"/>
+      <c r="G60" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
     </row>
     <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="29" t="str">
+      <c r="B61" s="26"/>
+      <c r="C61" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D61" s="28"/>
-      <c r="E61" s="30" t="str">
+      <c r="D61" s="26"/>
+      <c r="E61" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F61" s="28"/>
-      <c r="G61" s="30" t="str">
+      <c r="F61" s="26"/>
+      <c r="G61" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="28"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
     </row>
     <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B62" s="31"/>
-      <c r="C62" s="32" t="str">
+      <c r="B62" s="29"/>
+      <c r="C62" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D62" s="31"/>
-      <c r="E62" s="33" t="str">
+      <c r="D62" s="29"/>
+      <c r="E62" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F62" s="31"/>
-      <c r="G62" s="33" t="str">
+      <c r="F62" s="29"/>
+      <c r="G62" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-      <c r="J62" s="31"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
     </row>
     <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="28"/>
-      <c r="C63" s="29" t="str">
+      <c r="B63" s="26"/>
+      <c r="C63" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D63" s="28"/>
-      <c r="E63" s="30" t="str">
+      <c r="D63" s="26"/>
+      <c r="E63" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F63" s="28"/>
-      <c r="G63" s="30" t="str">
+      <c r="F63" s="26"/>
+      <c r="G63" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
-      <c r="J63" s="28"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
     </row>
     <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="31"/>
-      <c r="C64" s="32" t="str">
+      <c r="B64" s="29"/>
+      <c r="C64" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D64" s="31"/>
-      <c r="E64" s="33" t="str">
+      <c r="D64" s="29"/>
+      <c r="E64" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F64" s="31"/>
-      <c r="G64" s="33" t="str">
+      <c r="F64" s="29"/>
+      <c r="G64" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-      <c r="J64" s="31"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B65" s="28"/>
-      <c r="C65" s="29" t="str">
+      <c r="B65" s="26"/>
+      <c r="C65" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D65" s="28"/>
-      <c r="E65" s="30" t="str">
+      <c r="D65" s="26"/>
+      <c r="E65" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F65" s="28"/>
-      <c r="G65" s="30" t="str">
+      <c r="F65" s="26"/>
+      <c r="G65" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H65" s="28"/>
-      <c r="I65" s="28"/>
-      <c r="J65" s="28"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
     </row>
     <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="32" t="str">
+      <c r="B66" s="29"/>
+      <c r="C66" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D66" s="31"/>
-      <c r="E66" s="33" t="str">
+      <c r="D66" s="29"/>
+      <c r="E66" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F66" s="31"/>
-      <c r="G66" s="33" t="str">
+      <c r="F66" s="29"/>
+      <c r="G66" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
-      <c r="J66" s="31"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
     </row>
     <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B67" s="28"/>
-      <c r="C67" s="29" t="str">
+      <c r="B67" s="26"/>
+      <c r="C67" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D67" s="28"/>
-      <c r="E67" s="30" t="str">
+      <c r="D67" s="26"/>
+      <c r="E67" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F67" s="28"/>
-      <c r="G67" s="30" t="str">
+      <c r="F67" s="26"/>
+      <c r="G67" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="28"/>
+      <c r="H67" s="26"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="26"/>
     </row>
     <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B68" s="31"/>
-      <c r="C68" s="32" t="str">
+      <c r="B68" s="29"/>
+      <c r="C68" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D68" s="31"/>
-      <c r="E68" s="33" t="str">
+      <c r="D68" s="29"/>
+      <c r="E68" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F68" s="31"/>
-      <c r="G68" s="33" t="str">
+      <c r="F68" s="29"/>
+      <c r="G68" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H68" s="31"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="31"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
     </row>
     <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B69" s="28"/>
-      <c r="C69" s="29" t="str">
+      <c r="B69" s="26"/>
+      <c r="C69" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="30" t="str">
+      <c r="D69" s="26"/>
+      <c r="E69" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="30" t="str">
+      <c r="F69" s="26"/>
+      <c r="G69" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="26"/>
     </row>
     <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B70" s="31"/>
-      <c r="C70" s="32" t="str">
+      <c r="B70" s="29"/>
+      <c r="C70" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D70" s="31"/>
-      <c r="E70" s="33" t="str">
+      <c r="D70" s="29"/>
+      <c r="E70" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F70" s="31"/>
-      <c r="G70" s="33" t="str">
+      <c r="F70" s="29"/>
+      <c r="G70" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-      <c r="J70" s="31"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B71" s="28"/>
-      <c r="C71" s="29" t="str">
+      <c r="B71" s="26"/>
+      <c r="C71" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D71" s="28"/>
-      <c r="E71" s="30" t="str">
+      <c r="D71" s="26"/>
+      <c r="E71" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F71" s="28"/>
-      <c r="G71" s="30" t="str">
+      <c r="F71" s="26"/>
+      <c r="G71" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="28"/>
+      <c r="H71" s="26"/>
+      <c r="I71" s="26"/>
+      <c r="J71" s="26"/>
     </row>
     <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B72" s="31"/>
-      <c r="C72" s="32" t="str">
+      <c r="B72" s="29"/>
+      <c r="C72" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D72" s="31"/>
-      <c r="E72" s="33" t="str">
+      <c r="D72" s="29"/>
+      <c r="E72" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F72" s="31"/>
-      <c r="G72" s="33" t="str">
+      <c r="F72" s="29"/>
+      <c r="G72" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H72" s="31"/>
-      <c r="I72" s="31"/>
-      <c r="J72" s="31"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29"/>
     </row>
     <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B73" s="28"/>
-      <c r="C73" s="29" t="str">
+      <c r="B73" s="26"/>
+      <c r="C73" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D73" s="28"/>
-      <c r="E73" s="30" t="str">
+      <c r="D73" s="26"/>
+      <c r="E73" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F73" s="28"/>
-      <c r="G73" s="30" t="str">
+      <c r="F73" s="26"/>
+      <c r="G73" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="26"/>
     </row>
     <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="32" t="str">
+      <c r="B74" s="29"/>
+      <c r="C74" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D74" s="31"/>
-      <c r="E74" s="33" t="str">
+      <c r="D74" s="29"/>
+      <c r="E74" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F74" s="31"/>
-      <c r="G74" s="33" t="str">
+      <c r="F74" s="29"/>
+      <c r="G74" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H74" s="31"/>
-      <c r="I74" s="31"/>
-      <c r="J74" s="31"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="29"/>
     </row>
     <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B75" s="28"/>
-      <c r="C75" s="29" t="str">
+      <c r="B75" s="26"/>
+      <c r="C75" s="27" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D75" s="28"/>
-      <c r="E75" s="30" t="str">
+      <c r="D75" s="26"/>
+      <c r="E75" s="28" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F75" s="28"/>
-      <c r="G75" s="30" t="str">
+      <c r="F75" s="26"/>
+      <c r="G75" s="28" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="28"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="26"/>
+      <c r="J75" s="26"/>
     </row>
     <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B76" s="31"/>
-      <c r="C76" s="32" t="str">
+      <c r="B76" s="29"/>
+      <c r="C76" s="30" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="D76" s="31"/>
-      <c r="E76" s="33" t="str">
+      <c r="D76" s="29"/>
+      <c r="E76" s="31" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F76" s="31"/>
-      <c r="G76" s="33" t="str">
+      <c r="F76" s="29"/>
+      <c r="G76" s="31" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="H76" s="31"/>
-      <c r="I76" s="31"/>
-      <c r="J76" s="31"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
     </row>
     <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="s">

</xml_diff>